<commit_message>
Big and Small - Heaven and Hell 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Big and Small - Heaven and Hell - 3170117364/Big and Small - Heaven and Hell - 3170117364.xlsx
+++ b/Data/Big and Small - Heaven and Hell - 3170117364/Big and Small - Heaven and Hell - 3170117364.xlsx
@@ -1,26 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Big and Small - Heaven and Hell - 3170117364\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zilrt\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB5FB72-D810-4E15-9F3F-1EC2FAC1711C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206A6965-50A9-417F-82F2-463CE9F62580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2024-04-19_삭제된 노드 목록" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lammergeier</author>
+  </authors>
+  <commentList>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-04-19 이전의 원문: '[PAWN_nameDef] was doing middle-management within the divine hierarchy.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-04-19 이전의 원문: 'Carriers of this gene have a higher chance of becoming pregnant or impregnating others...'</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="350">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -55,18 +92,33 @@
     <t>BackstoryDef+BS_Unnatural.titleShort</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>언내추럴</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Unnatural.titleShort</t>
   </si>
   <si>
+    <t>BS_Unnatural.baseDesc</t>
+  </si>
+  <si>
     <t>BackstoryDef+BS_Unnatural.baseDesc</t>
   </si>
   <si>
-    <t>BS_Unnatural.baseDesc</t>
-  </si>
-  <si>
     <t>[PAWN_nameDef] was created by mysterious forces.</t>
   </si>
   <si>
+    <t>[PAWN_nameDef](은)는 정체불명의 힘에 의해 만들어졌습니다.</t>
+  </si>
+  <si>
     <t>BackstoryDef+BS_HeavenServitor.title</t>
   </si>
   <si>
@@ -79,6 +131,18 @@
     <t>BackstoryDef+BS_HeavenServitor.titleShort</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>천상의 종</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_HeavenServitor.titleShort</t>
   </si>
   <si>
@@ -88,12 +152,21 @@
     <t>BackstoryDef+BS_HeavenServitor.baseDesc</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>종</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_HeavenServitor.baseDesc</t>
   </si>
   <si>
-    <t>[PAWN_nameDef] was doing middle-management within the divine hierarchy.</t>
-  </si>
-  <si>
     <t>BackstoryDef+BS_HeavenWarrior.title</t>
   </si>
   <si>
@@ -103,12 +176,39 @@
     <t>BackstoryDef+BS_HeavenWarrior.titleShort</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>heavenly warrior</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>천상의 전사</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_HeavenWarrior.titleShort</t>
   </si>
   <si>
     <t>warrior</t>
   </si>
   <si>
+    <t>전사</t>
+  </si>
+  <si>
     <t>BackstoryDef+BS_HeavenWarrior.baseDesc</t>
   </si>
   <si>
@@ -118,6 +218,9 @@
     <t>[PAWN_nameDef]'s main duty was that of a heavenly warrior.</t>
   </si>
   <si>
+    <t>[PAWN_nameDef]의 주요 임무는 천상의 전사였습니다.</t>
+  </si>
+  <si>
     <t>BackstoryDef+BS_Satan.title</t>
   </si>
   <si>
@@ -130,18 +233,33 @@
     <t>BackstoryDef+BS_Satan.titleShort</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>대적자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Satan.titleShort</t>
   </si>
   <si>
+    <t>BS_Satan.baseDesc</t>
+  </si>
+  <si>
     <t>BackstoryDef+BS_Satan.baseDesc</t>
   </si>
   <si>
-    <t>BS_Satan.baseDesc</t>
-  </si>
-  <si>
     <t>[PAWN_nameDef]'s main duty was to test the faithful and judge the guilty.</t>
   </si>
   <si>
+    <t>[PAWN_nameDef]의 주요 임무는 신자들을 시험하고 유죄를 판단하는 것이었습니다.</t>
+  </si>
+  <si>
     <t>FactionDef+BS_Heaven.label</t>
   </si>
   <si>
@@ -157,18 +275,57 @@
     <t>FactionDef+BS_Heaven.fixedName</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>디바인 렐름</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Heaven.fixedName</t>
   </si>
   <si>
     <t>FactionDef+BS_Heaven.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>Kingdom of Heaven</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>하늘의 왕국</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Heaven.description</t>
   </si>
   <si>
     <t>When the time of judgement comes all siners shall be cleansed in the flames of purgatory.</t>
   </si>
   <si>
+    <t>심판의 때가 오면 모든 죄인은 연옥의 불길 속에서 깨끗하게 씻겨질 것입니다.</t>
+  </si>
+  <si>
     <t>FactionDef+BS_Heaven.pawnSingular</t>
   </si>
   <si>
@@ -181,6 +338,18 @@
     <t>FactionDef+BS_Heaven.pawnsPlural</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>메신저</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Heaven.pawnsPlural</t>
   </si>
   <si>
@@ -190,12 +359,27 @@
     <t>FactionDef+BS_Heaven.leaderTitle</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>메신저들</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Heaven.leaderTitle</t>
   </si>
   <si>
     <t>voice of the creator</t>
   </si>
   <si>
+    <t>창조주의 목소리</t>
+  </si>
+  <si>
     <t>FactionDef+BS_Hell.label</t>
   </si>
   <si>
@@ -208,12 +392,27 @@
     <t>FactionDef+BS_Hell.fixedName</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>인페르날 렐름</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Hell.fixedName</t>
   </si>
   <si>
     <t>Tyrany of Hell</t>
   </si>
   <si>
+    <t>지옥의 폭군</t>
+  </si>
+  <si>
     <t>FactionDef+BS_Hell.leaderTitle</t>
   </si>
   <si>
@@ -226,12 +425,27 @@
     <t>FactionDef+BS_Hell.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>군주</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Hell.description</t>
   </si>
   <si>
     <t>The realms appear fairly independent from each other and usually ruled by some sort of demon lord.</t>
   </si>
   <si>
+    <t>이 왕국들은 서로 상당히 독립적으로 보이며, 보통 일종의 악마 군주가 통치합니다.</t>
+  </si>
+  <si>
     <t>FactionDef+BS_Hell.pawnSingular</t>
   </si>
   <si>
@@ -244,6 +458,18 @@
     <t>FactionDef+BS_Hell.pawnsPlural</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>악마</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Hell.pawnsPlural</t>
   </si>
   <si>
@@ -253,6 +479,18 @@
     <t>FactionDef+BS_Outcasts.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>악마들</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Outcasts.label</t>
   </si>
   <si>
@@ -262,6 +500,18 @@
     <t>FactionDef+BS_Outcasts.fixedName</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>외계 추방자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Outcasts.fixedName</t>
   </si>
   <si>
@@ -271,12 +521,27 @@
     <t>FactionDef+BS_Outcasts.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>독립자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Outcasts.description</t>
   </si>
   <si>
     <t>A seemingly disorganized group of outcasts led by fallen angels.</t>
   </si>
   <si>
+    <t>타락한 천사들이 이끄는 겉보기에는 무질서한 추방자 집단입니다.</t>
+  </si>
+  <si>
     <t>FactionDef+BS_Outcasts.pawnSingular</t>
   </si>
   <si>
@@ -286,6 +551,9 @@
     <t>outcast</t>
   </si>
   <si>
+    <t>추방자</t>
+  </si>
+  <si>
     <t>FactionDef+BS_Outcasts.pawnsPlural</t>
   </si>
   <si>
@@ -298,6 +566,18 @@
     <t>FactionDef+BS_Outcasts.leaderTitle</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>추방자들</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Outcasts.leaderTitle</t>
   </si>
   <si>
@@ -307,6 +587,18 @@
     <t>GeneDef+BS_AngelHalo.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>지도자</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GeneDef</t>
   </si>
   <si>
@@ -316,6 +608,9 @@
     <t>angelic halo</t>
   </si>
   <si>
+    <t>천사의 후광</t>
+  </si>
+  <si>
     <t>GeneDef+BS_AngelHalo.description</t>
   </si>
   <si>
@@ -325,6 +620,9 @@
     <t>Carriers of this gene possess an angelic halo.</t>
   </si>
   <si>
+    <t>이 유전자의 보유자는 천사의 후광을 가지고 있습니다.</t>
+  </si>
+  <si>
     <t>GeneDef+BS_FalseHalo.label</t>
   </si>
   <si>
@@ -334,6 +632,9 @@
     <t>false halo</t>
   </si>
   <si>
+    <t>거짓 후광</t>
+  </si>
+  <si>
     <t>GeneDef+BS_FalseHalo.description</t>
   </si>
   <si>
@@ -343,6 +644,9 @@
     <t>Carriers of this gene possess a strange halo.</t>
   </si>
   <si>
+    <t>이 유전자의 보유자는 이상한 후광을 가지고 있습니다.</t>
+  </si>
+  <si>
     <t>GeneDef+BS_FieryHalo.label</t>
   </si>
   <si>
@@ -352,6 +656,9 @@
     <t>burning halo</t>
   </si>
   <si>
+    <t>불타는 후광</t>
+  </si>
+  <si>
     <t>GeneDef+BS_FieryHalo.description</t>
   </si>
   <si>
@@ -361,6 +668,9 @@
     <t>Carriers of this gene possess an burning angelic halo.</t>
   </si>
   <si>
+    <t>이 유전자의 보유자는 불타는 천사의 후광을 가지고 있습니다.</t>
+  </si>
+  <si>
     <t>GeneDef+BS_MenacingHalo.label</t>
   </si>
   <si>
@@ -370,6 +680,9 @@
     <t>meanacing halo</t>
   </si>
   <si>
+    <t>위협적인 후광</t>
+  </si>
+  <si>
     <t>GeneDef+BS_MenacingHalo.description</t>
   </si>
   <si>
@@ -379,6 +692,9 @@
     <t>Carriers of this gene possess an menacing dark halo.</t>
   </si>
   <si>
+    <t>이 유전자의 보유자는 위협적인 어두운 후광을 가지고 있습니다.</t>
+  </si>
+  <si>
     <t>GeneDef+BS_GrigoriFertile.label</t>
   </si>
   <si>
@@ -391,12 +707,21 @@
     <t>GeneDef+BS_GrigoriFertile.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>다산</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_GrigoriFertile.description</t>
   </si>
   <si>
-    <t>Carriers of this gene have a higher chance of becoming pregnant or impregnating others...</t>
-  </si>
-  <si>
     <t>PawnKindDef+BS_ServitorBasic.label</t>
   </si>
   <si>
@@ -409,6 +734,9 @@
     <t>holy servitor</t>
   </si>
   <si>
+    <t>거룩한 종</t>
+  </si>
+  <si>
     <t>PawnKindDef+BS_ServitorMelee.label</t>
   </si>
   <si>
@@ -430,6 +758,9 @@
     <t>holy archer</t>
   </si>
   <si>
+    <t>거룩한 궁수</t>
+  </si>
+  <si>
     <t>PawnKindDef+BS_Satan.label</t>
   </si>
   <si>
@@ -439,6 +770,9 @@
     <t>angel of hell</t>
   </si>
   <si>
+    <t>지옥의 천사</t>
+  </si>
+  <si>
     <t>PawnKindDef+BS_SatanLimited.label</t>
   </si>
   <si>
@@ -454,6 +788,9 @@
     <t>great satan</t>
   </si>
   <si>
+    <t>위대한 사탄</t>
+  </si>
+  <si>
     <t>PawnKindDef+BS_AuthorityWarrior.label</t>
   </si>
   <si>
@@ -463,6 +800,9 @@
     <t>holy warrior</t>
   </si>
   <si>
+    <t>거룩한 전사</t>
+  </si>
+  <si>
     <t>PawnKindDef+BS_AuthorityLord.label</t>
   </si>
   <si>
@@ -475,12 +815,27 @@
     <t>PawnKindDef+BS_Metatron.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>위대한 권능</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Metatron.label</t>
   </si>
   <si>
     <t>voice of god</t>
   </si>
   <si>
+    <t>신의 목소리</t>
+  </si>
+  <si>
     <t>PawnKindDef+BS_NephilimWarrior.label</t>
   </si>
   <si>
@@ -499,6 +854,18 @@
     <t>PawnKindDef+BS_SmallGlutton.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>식탐의 악마</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_SmallGlutton.label</t>
   </si>
   <si>
@@ -508,6 +875,18 @@
     <t>PawnKindDef+VU_LilimWarrior.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>작은 식탐의 악마</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>VU_LilimWarrior.label</t>
   </si>
   <si>
@@ -517,6 +896,18 @@
     <t>XenotypeDef+BS_Authority.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>헬가드</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>XenotypeDef</t>
   </si>
   <si>
@@ -529,12 +920,27 @@
     <t>XenotypeDef+BS_Authority.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>권능</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Authority.description</t>
   </si>
   <si>
     <t>Incredibly powerful angels most commonly seen on the battlefield. Not much is known about them beyond the fact that they are very high-ranked in the divine hierarchy.</t>
   </si>
   <si>
+    <t>전장에서 가장 흔히 볼 수 있는 놀랍도록 강력한 천사. 신성 서열에서 매우 높은 지위에 있다는 사실 외에는 알려진 바가 많지 않습니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Authority.descriptionShort</t>
   </si>
   <si>
@@ -544,6 +950,9 @@
     <t>Incredibly powerful angels most commonly seen on the battlefield.</t>
   </si>
   <si>
+    <t>전장에서 가장 흔히 볼 수 있는 놀랍도록 강력한 천사들입니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Malakim.label</t>
   </si>
   <si>
@@ -556,12 +965,27 @@
     <t>XenotypeDef+BS_Malakim.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>말라킴</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Malakim.description</t>
   </si>
   <si>
     <t>Also known as messengers, the Malakim are the most often seen among the angels and they do much of the busywork in Heaven. Contrary to what many believe Malakim like most angels fundamentally fail to understand how humans think and are terrible at communicating anything more complex than basic messages or commands, sometimes failing at even that...\n\n"Faithful followers BEWARE. This city has been found wanting on the eve of winter it faces judgement."\n\n"...and after saying so it left. So, uh, wanting how? Does it mean we must improve the homeless situation? Convert the faithless? Quickly evacuate the city? ...All of the above?"</t>
   </si>
   <si>
+    <t>메신저라고도 알려진 말라킴은 천사들 중에서 가장 자주 볼 수 있으며 천국에서 바쁜 일을 많이 합니다. 많은 사람들이 생각하는 것과는 달리 말라킴은 대부분의 천사들과 마찬가지로 인간의 사고 방식을 근본적으로 이해하지 못하며 기본적인 메시지나 명령보다 더 복잡한 것을 전달하는 데 끔찍하게 실패하며 때로는 그조차도 실패합니다....\n\n"신실한 추종자들은 조심하라. 이 도시는 겨울이 오기 직전에 심판을 받게 될 것이다."\n\n"...그리고 그렇게 말한 후 떠났어. 그래서, 어쩌라고? 노숙자 상황을 개선해야 한다는 뜻인가? 믿지 않는 사람들을 개종시키라는 건가? 사람들을 도시에서 빨리 대피시키라는 건가? ... 아니면 전부?"</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Malakim.descriptionShort</t>
   </si>
   <si>
@@ -571,6 +995,9 @@
     <t>Malakim are the most common among the angels. They often act as messengers.</t>
   </si>
   <si>
+    <t>말라킴은 천사 중에서 가장 흔한 천사입니다. 그들은 종종 메신저 역할을 합니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Satan.label</t>
   </si>
   <si>
@@ -580,12 +1007,27 @@
     <t>XenotypeDef+BS_Satan.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>사탄</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Satan.description</t>
   </si>
   <si>
     <t>Also known as the Angels of Hell, Adversaries, or Zabaniyah. Satans are said to be angels tasked with testing worth by means of taunting, inflicting suffering, and tempting humanity with sin. They are sometimes said to have some responsibility to punish sinners and control Hell.\n\nPerhaps because of their nature as designated adversaries they are among the few angels that seem to understand humans. Despite their frightening appearance and sometime even crueler acts, there are some cults claiming that the Satans generally sympathise and ultimately wish the best for humanity, more so than any other angels.</t>
   </si>
   <si>
+    <t>지옥의 천사, 대적자 또는 자바니야라고도 합니다. 사탄은 인간을 조롱하고 고통을 가하며 죄로 유혹하여 가치를 시험하는 임무를 맡은 천사라고 알려져 있습니다. 그들은 때때로 죄인을 벌하고 지옥을 통제할 책임이 있다고도 합니다.\n\n대적자라는 성격 때문인지 그들은 인간을 이해하는 몇 안 되는 천사 중 하나입니다. 무서운 외모와 때로는 잔인한 행동에도 불구하고 사탄은 일반적으로 다른 어떤 천사보다 인간을 동정하고 궁극적으로 인간을 위해 최선을 다한다고 주장하는 일부 종파가 있습니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Satan.descriptionShort</t>
   </si>
   <si>
@@ -595,6 +1037,9 @@
     <t>Also known as the Angels of Hell or Zabaniyah.</t>
   </si>
   <si>
+    <t>지옥의 천사 또는 자바니야라고도 합니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Grigori.label</t>
   </si>
   <si>
@@ -604,6 +1049,9 @@
     <t>Grigori</t>
   </si>
   <si>
+    <t>그리고리</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Grigori.description</t>
   </si>
   <si>
@@ -613,6 +1061,9 @@
     <t>Also known as the Fallen Watchers. Grigori are outcasts amongst angels, considered by many to be worse than even demons, these angels were allegedly tasked with watching over and guiding humanity. It is said that they were much more capable of understanding and connecting with humans than other angels. Reportedly a more humanlike nature was their downfall, as stories speak of the grigori teaching forbidden secrets and even coupling with humans; birthing the savage titans known as Nephilim.</t>
   </si>
   <si>
+    <t>타락한 감시자라고도 합니다. 그리고리는 천사들 사이에서 버림받은 존재로, 악마보다 더한 존재로 여겨지며 인류를 감시하고 인도하는 임무를 맡았다고 합니다. 다른 천사들보다 인간을 이해하고 인간과 소통하는 능력이 훨씬 뛰어났다고 합니다. 그리고리가 금지된 비밀을 가르치고 심지어 인간과 결합하여 네피림으로 알려진 야만적인 거인들을 낳았다는 이야기에서 알 수 있듯이, 인간과 더 닮은 본성이 그들의 몰락을 가져왔다고 전해집니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Grigori.descriptionShort</t>
   </si>
   <si>
@@ -622,6 +1073,9 @@
     <t>Also known as the Fallen Watchers, they are the angels who were responsible for watching over humans.</t>
   </si>
   <si>
+    <t>타락한 감시자라고도 불리는 이들은 인간을 감시하는 일을 담당했던 천사입니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Glutton.label</t>
   </si>
   <si>
@@ -634,6 +1088,18 @@
     <t>XenotypeDef+BS_Glutton.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>글루톤</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Glutton.description</t>
   </si>
   <si>
@@ -643,12 +1109,27 @@
     <t>XenotypeDef+BS_Glutton.descriptionShort</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>글루톤은 이빨과 입으로 뒤덮인 무시무시한 악마입니다. 전투 중에도 적을 잡아먹는 것을 멈추지 못합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Glutton.descriptionShort</t>
   </si>
   <si>
     <t>Gluttons are terrifying demons covered in teeth and mouths.</t>
   </si>
   <si>
+    <t>글루톤은 이빨과 입으로 뒤덮인 무시무시한 악마입니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_LilGlutton.label</t>
   </si>
   <si>
@@ -661,6 +1142,18 @@
     <t>XenotypeDef+BS_LilGlutton.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>작은 글루톤</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_LilGlutton.description</t>
   </si>
   <si>
@@ -670,6 +1163,18 @@
     <t>XenotypeDef+BS_Nephilim.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>작은 글루톤은 글루톤의 작은 버전으로 보입니다. 이들도 덩치가 큰 종족과 마찬가지로 탐욕스러운 식욕을 가지고 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Nephilim.label</t>
   </si>
   <si>
@@ -679,6 +1184,18 @@
     <t>XenotypeDef+BS_Nephilim.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>네피림</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Nephilim.description</t>
   </si>
   <si>
@@ -688,12 +1205,27 @@
     <t>XenotypeDef+BS_Nephilim.descriptionShort</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>네피림은 그리고리와 인간이 낳은 기괴하고 거대한 자손으로 알려져 있습니다. 천사들은 네피림을 인간을 닮은 가장 부자연스럽고 더러운 식인 괴물이라고 묘사합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Nephilim.descriptionShort</t>
   </si>
   <si>
     <t>Nephilim are said to be grotesquely enormus offspring of a Grigori and a human</t>
   </si>
   <si>
+    <t>네피림은 그리고리와 인간이 낳은 기괴하고 거대한 자손으로 알려져 있습니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Lilim.label</t>
   </si>
   <si>
@@ -706,21 +1238,147 @@
     <t>XenotypeDef+BS_Lilim.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>릴림</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Lilim.description</t>
   </si>
   <si>
     <t>Lilim; sometimes called lili if female or lilu if male; are sometimes said to be the offspring or descendants of the mythical Lilith. According to legend Lilith would bed fallen angels and demons and these unions produced many children.\n\nLilim in particular are said to be jealous, lustful, and dangerous especially to the spouse and children of a person they've taken interest in.</t>
   </si>
   <si>
+    <t>여성인 경우 릴리, 남성인 경우 릴루라고도 불리는 릴림은 신화 속 릴리스의 자손 또는 후손이라고도 합니다. 전설에 따르면 릴리스는 타락한 천사와 악마와 동침했으며, 이 결합으로 많은 아이를 낳았다고 합니다.\n\n특히 릴림은 질투심과 정욕이 강하고 특히 관심을 가진 사람의 배우자와 자녀에게 위험한 것으로 알려져 있습니다.</t>
+  </si>
+  <si>
     <t>XenotypeDef+BS_Lilim.descriptionShort</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>XenotypeDef</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>BS_Lilim.descriptionShort</t>
   </si>
   <si>
     <t>According to legends these are among the many offspring of the mythical Lilith.</t>
   </si>
   <si>
+    <t>전설에 따르면 이들은 신화 속 릴리스의 수많은 자손 중 하나라고 합니다.</t>
+  </si>
+  <si>
+    <t>VU_Succubus.label</t>
+  </si>
+  <si>
+    <t>Succubus</t>
+  </si>
+  <si>
+    <t>VU_Succubus.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>서큐버스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Succubus/Incubus are said to be demons that seduce their victims and prey upon them and the victim's friends and family.</t>
+  </si>
+  <si>
+    <t>서큐버스/인큐버스는 피해자를 유혹하여 피해자와 피해자의 친구 및 가족을 잡아먹는 악마로 알려져 있습니다.</t>
+  </si>
+  <si>
+    <t>VU_Hellguard.label</t>
+  </si>
+  <si>
+    <t>Hellguard</t>
+  </si>
+  <si>
+    <t>These large creatures are the backbone of the hells' armies and their industry</t>
+  </si>
+  <si>
+    <t>VU_Hellguard.description</t>
+  </si>
+  <si>
+    <t>이 거대한 생명체는 지옥의 군대와 산업의 중추입니다.</t>
+  </si>
+  <si>
+    <t>VU_Gatekeeper.label</t>
+  </si>
+  <si>
+    <t>Gatekeeper</t>
+  </si>
+  <si>
+    <t>VU_Gatekeeper.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>게이트키퍼</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>These lumbering creatures are often found guarding important sites.</t>
+  </si>
+  <si>
+    <t>이 덩치 큰 생명체는 종종 중요한 장소를 지키는 모습을 볼 수 있습니다.</t>
+  </si>
+  <si>
+    <t>VU_Imp.label</t>
+  </si>
+  <si>
+    <t>Imp</t>
+  </si>
+  <si>
+    <t>VU_Imp.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>임프</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>These little theives are often in all sorts of strange places. They are especially know for stealing technological gadgets.</t>
+  </si>
+  <si>
+    <t>이 작은 도둑들은 종종 온갖 이상한 장소에 숨어 있습니다. 특히 기술 기기를 훔치는 것으로 유명합니다.</t>
+  </si>
+  <si>
     <t>PawnKindDef+VU_ImpFighter.label</t>
   </si>
   <si>
@@ -733,21 +1391,45 @@
     <t>PawnKindDef+VU_DemonWarrior.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>페스트</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>VU_DemonWarrior.label</t>
   </si>
   <si>
+    <t>VU_DemonCommander.label</t>
+  </si>
+  <si>
     <t>PawnKindDef+VU_DemonCommander.label</t>
   </si>
   <si>
-    <t>VU_DemonCommander.label</t>
-  </si>
-  <si>
     <t>commander</t>
   </si>
   <si>
     <t>PawnKindDef+VU_DemonCommander_Suc.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>커맨더</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>VU_DemonCommander_Suc.label</t>
   </si>
   <si>
@@ -757,360 +1439,54 @@
     <t>PawnKindDef+VU_DemonBrute.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>노블</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>VU_DemonBrute.label</t>
   </si>
   <si>
     <t>gatekeeper</t>
   </si>
   <si>
-    <t>언내추럴</t>
+    <t>Carriers of this gene have a higher chance of becoming pregnant or impregnating others...\n\nThere is something wrong with this gene. Best be careful.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>[PAWN_nameDef](은)는 정체불명의 힘에 의해 만들어졌습니다.</t>
-  </si>
-  <si>
-    <t>종</t>
+    <t>이 유전자의 보유자는 임신하거나 다른 사람을 임신시킬 확률이 더 높습니다...\n\n이 유전자에 문제가 있습니다. 조심해야 합니다.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>[PAWN_nameDef] was doing middle-management within the divine hierarchy, with a side of smiting.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>heavenly warrior</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>천상의 종</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>천상의 전사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>전사</t>
-  </si>
-  <si>
-    <t>[PAWN_nameDef]의 주요 임무는 신자들을 시험하고 유죄를 판단하는 것이었습니다.</t>
-  </si>
-  <si>
-    <t>[PAWN_nameDef]의 주요 임무는 천상의 전사였습니다.</t>
-  </si>
-  <si>
-    <t>디바인 렐름</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kingdom of Heaven</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>하늘의 왕국</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>심판의 때가 오면 모든 죄인은 연옥의 불길 속에서 깨끗하게 씻겨질 것입니다.</t>
-  </si>
-  <si>
-    <t>메신저</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>메신저들</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>창조주의 목소리</t>
-  </si>
-  <si>
-    <t>인페르날 렐름</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지옥의 폭군</t>
-  </si>
-  <si>
-    <t>군주</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 왕국들은 서로 상당히 독립적으로 보이며, 보통 일종의 악마 군주가 통치합니다.</t>
-  </si>
-  <si>
-    <t>악마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>악마들</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>독립자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>타락한 천사들이 이끄는 겉보기에는 무질서한 추방자 집단입니다.</t>
-  </si>
-  <si>
-    <t>외계 추방자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>추방자</t>
-  </si>
-  <si>
-    <t>추방자들</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지도자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>천사의 후광</t>
-  </si>
-  <si>
-    <t>이 유전자의 보유자는 천사의 후광을 가지고 있습니다.</t>
-  </si>
-  <si>
-    <t>거짓 후광</t>
-  </si>
-  <si>
-    <t>이 유전자의 보유자는 이상한 후광을 가지고 있습니다.</t>
-  </si>
-  <si>
-    <t>불타는 후광</t>
-  </si>
-  <si>
-    <t>이 유전자의 보유자는 불타는 천사의 후광을 가지고 있습니다.</t>
-  </si>
-  <si>
-    <t>위협적인 후광</t>
-  </si>
-  <si>
-    <t>이 유전자의 보유자는 위협적인 어두운 후광을 가지고 있습니다.</t>
-  </si>
-  <si>
-    <t>이 유전자의 보유자는 임신하거나 다른 사람을 임신시킬 확률이 더 높습니다 ...</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다산</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>거룩한 종</t>
-  </si>
-  <si>
-    <t>거룩한 궁수</t>
-  </si>
-  <si>
-    <t>지옥의 천사</t>
-  </si>
-  <si>
-    <t>위대한 사탄</t>
-  </si>
-  <si>
-    <t>거룩한 전사</t>
-  </si>
-  <si>
-    <t>신의 목소리</t>
-  </si>
-  <si>
-    <t>식탐의 악마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작은 식탐의 악마</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>헬가드</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>권능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>위대한 권능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[PAWN_nameDef](은)는 신성 서열 내에서 중간 관리를 하고 있었습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>전장에서 가장 흔히 볼 수 있는 놀랍도록 강력한 천사. 신성 서열에서 매우 높은 지위에 있다는 사실 외에는 알려진 바가 많지 않습니다.</t>
-  </si>
-  <si>
-    <t>전장에서 가장 흔히 볼 수 있는 놀랍도록 강력한 천사들입니다.</t>
-  </si>
-  <si>
-    <t>말라킴</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>메신저라고도 알려진 말라킴은 천사들 중에서 가장 자주 볼 수 있으며 천국에서 바쁜 일을 많이 합니다. 많은 사람들이 생각하는 것과는 달리 말라킴은 대부분의 천사들과 마찬가지로 인간의 사고 방식을 근본적으로 이해하지 못하며 기본적인 메시지나 명령보다 더 복잡한 것을 전달하는 데 끔찍하게 실패하며 때로는 그조차도 실패합니다....\n\n"신실한 추종자들은 조심하라. 이 도시는 겨울이 오기 직전에 심판을 받게 될 것이다."\n\n"...그리고 그렇게 말한 후 떠났어. 그래서, 어쩌라고? 노숙자 상황을 개선해야 한다는 뜻인가? 믿지 않는 사람들을 개종시키라는 건가? 사람들을 도시에서 빨리 대피시키라는 건가? ... 아니면 전부?"</t>
-  </si>
-  <si>
-    <t>말라킴은 천사 중에서 가장 흔한 천사입니다. 그들은 종종 메신저 역할을 합니다.</t>
-  </si>
-  <si>
-    <t>사탄</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>대적자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지옥의 천사, 대적자 또는 자바니야라고도 합니다. 사탄은 인간을 조롱하고 고통을 가하며 죄로 유혹하여 가치를 시험하는 임무를 맡은 천사라고 알려져 있습니다. 그들은 때때로 죄인을 벌하고 지옥을 통제할 책임이 있다고도 합니다.\n\n대적자라는 성격 때문인지 그들은 인간을 이해하는 몇 안 되는 천사 중 하나입니다. 무서운 외모와 때로는 잔인한 행동에도 불구하고 사탄은 일반적으로 다른 어떤 천사보다 인간을 동정하고 궁극적으로 인간을 위해 최선을 다한다고 주장하는 일부 종파가 있습니다.</t>
-  </si>
-  <si>
-    <t>지옥의 천사 또는 자바니야라고도 합니다.</t>
-  </si>
-  <si>
-    <t>그리고리</t>
-  </si>
-  <si>
-    <t>타락한 감시자라고도 합니다. 그리고리는 천사들 사이에서 버림받은 존재로, 악마보다 더한 존재로 여겨지며 인류를 감시하고 인도하는 임무를 맡았다고 합니다. 다른 천사들보다 인간을 이해하고 인간과 소통하는 능력이 훨씬 뛰어났다고 합니다. 그리고리가 금지된 비밀을 가르치고 심지어 인간과 결합하여 네피림으로 알려진 야만적인 거인들을 낳았다는 이야기에서 알 수 있듯이, 인간과 더 닮은 본성이 그들의 몰락을 가져왔다고 전해집니다.</t>
-  </si>
-  <si>
-    <t>타락한 감시자라고도 불리는 이들은 인간을 감시하는 일을 담당했던 천사입니다.</t>
-  </si>
-  <si>
-    <t>글루톤</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>글루톤은 이빨과 입으로 뒤덮인 무시무시한 악마입니다. 전투 중에도 적을 잡아먹는 것을 멈추지 못합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>글루톤은 이빨과 입으로 뒤덮인 무시무시한 악마입니다.</t>
-  </si>
-  <si>
-    <t>작은 글루톤</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작은 글루톤은 글루톤의 작은 버전으로 보입니다. 이들도 덩치가 큰 종족과 마찬가지로 탐욕스러운 식욕을 가지고 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>네피림</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>네피림은 그리고리와 인간이 낳은 기괴하고 거대한 자손으로 알려져 있습니다. 천사들은 네피림을 인간을 닮은 가장 부자연스럽고 더러운 식인 괴물이라고 묘사합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>네피림은 그리고리와 인간이 낳은 기괴하고 거대한 자손으로 알려져 있습니다.</t>
-  </si>
-  <si>
-    <t>릴림</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>여성인 경우 릴리, 남성인 경우 릴루라고도 불리는 릴림은 신화 속 릴리스의 자손 또는 후손이라고도 합니다. 전설에 따르면 릴리스는 타락한 천사와 악마와 동침했으며, 이 결합으로 많은 아이를 낳았다고 합니다.\n\n특히 릴림은 질투심과 정욕이 강하고 특히 관심을 가진 사람의 배우자와 자녀에게 위험한 것으로 알려져 있습니다.</t>
-  </si>
-  <si>
-    <t>전설에 따르면 이들은 신화 속 릴리스의 수많은 자손 중 하나라고 합니다.</t>
-  </si>
-  <si>
-    <t>페스트</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>커맨더</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>노블</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>게이트키퍼</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XenotypeDef</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>VU_Succubus.label</t>
-  </si>
-  <si>
-    <t>VU_Succubus.description</t>
-  </si>
-  <si>
-    <t>VU_Hellguard.label</t>
-  </si>
-  <si>
-    <t>VU_Hellguard.description</t>
-  </si>
-  <si>
-    <t>VU_Gatekeeper.label</t>
-  </si>
-  <si>
-    <t>VU_Gatekeeper.description</t>
-  </si>
-  <si>
-    <t>VU_Imp.label</t>
-  </si>
-  <si>
-    <t>VU_Imp.description</t>
-  </si>
-  <si>
-    <t>Succubus</t>
-  </si>
-  <si>
-    <t>Succubus/Incubus are said to be demons that seduce their victims and prey upon them and the victim's friends and family.</t>
-  </si>
-  <si>
-    <t>Hellguard</t>
-  </si>
-  <si>
-    <t>These large creatures are the backbone of the hells' armies and their industry</t>
-  </si>
-  <si>
-    <t>Gatekeeper</t>
-  </si>
-  <si>
-    <t>These lumbering creatures are often found guarding important sites.</t>
-  </si>
-  <si>
-    <t>Imp</t>
-  </si>
-  <si>
-    <t>These little theives are often in all sorts of strange places. They are especially know for stealing technological gadgets.</t>
-  </si>
-  <si>
-    <t>서큐버스</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>서큐버스/인큐버스는 피해자를 유혹하여 피해자와 피해자의 친구 및 가족을 잡아먹는 악마로 알려져 있습니다.</t>
-  </si>
-  <si>
-    <t>이 거대한 생명체는 지옥의 군대와 산업의 중추입니다.</t>
-  </si>
-  <si>
-    <t>이 덩치 큰 생명체는 종종 중요한 장소를 지키는 모습을 볼 수 있습니다.</t>
-  </si>
-  <si>
-    <t>임프</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 작은 도둑들은 종종 온갖 이상한 장소에 숨어 있습니다. 특히 기술 기기를 훔치는 것으로 유명합니다.</t>
+    <t>[PAWN_nameDef](은)는 신성 서열 내에서 중간 관리를 하고 있었으며, 벌을 내리기도 했습니다.</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS_Unnatural.description</t>
+  </si>
+  <si>
+    <t>BS_HeavenServitor.description</t>
+  </si>
+  <si>
+    <t>BS_HeavenWarrior.description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1129,13 +1505,24 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1150,9 +1537,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1454,14 +1842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" style="1" customWidth="1"/>
@@ -1507,7 +1895,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>247</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1518,18 +1906,18 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>247</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -1538,1465 +1926,1556 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>248</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>251</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>249</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>296</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>250</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>252</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>253</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>255</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>303</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>303</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>254</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>256</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>257</v>
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>258</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>259</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>260</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>261</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>262</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>263</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>264</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>265</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>266</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>267</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>268</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>271</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>269</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>270</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>272</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>273</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>274</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>275</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>276</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>277</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>278</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>279</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>280</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>281</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>284</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>124</v>
+        <v>160</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>283</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>285</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>285</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>285</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>286</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>287</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>287</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>288</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>289</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>295</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>290</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>154</v>
+        <v>197</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>289</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>291</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>160</v>
+        <v>204</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>292</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>161</v>
+        <v>205</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>162</v>
+        <v>207</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>293</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>294</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>170</v>
+        <v>217</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>297</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>173</v>
+        <v>221</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>298</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>299</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>300</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>180</v>
+        <v>231</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>181</v>
+        <v>232</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>301</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>183</v>
+        <v>235</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>184</v>
+        <v>236</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>302</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>185</v>
+        <v>237</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>187</v>
+        <v>240</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>304</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>188</v>
+        <v>242</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>190</v>
+        <v>244</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>305</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>191</v>
+        <v>246</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>192</v>
+        <v>247</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>306</v>
+        <v>249</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>194</v>
+        <v>250</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>307</v>
+        <v>253</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>197</v>
+        <v>254</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>308</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>200</v>
+        <v>258</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>202</v>
+        <v>260</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>309</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>203</v>
+        <v>261</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>204</v>
+        <v>263</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>205</v>
+        <v>264</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>206</v>
+        <v>265</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>208</v>
+        <v>268</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>311</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>209</v>
+        <v>270</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>210</v>
+        <v>271</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>213</v>
+        <v>275</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>216</v>
+        <v>279</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>217</v>
+        <v>280</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>218</v>
+        <v>281</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>219</v>
+        <v>283</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>220</v>
+        <v>284</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>315</v>
+        <v>286</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>221</v>
+        <v>285</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>222</v>
+        <v>287</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>223</v>
+        <v>288</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>224</v>
+        <v>290</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>225</v>
+        <v>291</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>226</v>
+        <v>292</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>227</v>
+        <v>293</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>228</v>
+        <v>295</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>230</v>
+        <v>298</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>232</v>
+        <v>301</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>341</v>
+        <v>306</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>342</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>293</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>336</v>
+        <v>311</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>344</v>
+        <v>319</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>233</v>
+        <v>326</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>234</v>
+        <v>327</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>235</v>
+        <v>328</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>236</v>
+        <v>329</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>237</v>
+        <v>331</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>293</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>238</v>
+        <v>333</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>239</v>
+        <v>332</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>240</v>
+        <v>334</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>241</v>
+        <v>335</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>242</v>
+        <v>337</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>243</v>
+        <v>338</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>322</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>244</v>
+        <v>339</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>245</v>
+        <v>341</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>246</v>
+        <v>342</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B96" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>